<commit_message>
Merging my github files from PC to USB
</commit_message>
<xml_diff>
--- a/documentation/BudgetPlan.xlsx
+++ b/documentation/BudgetPlan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n01114847\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ceng317\SensorEffector\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,75 +24,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Link</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
-    <t>CAD$ Unit Cost</t>
-  </si>
-  <si>
     <t>Total for parts from CAD sources</t>
   </si>
   <si>
-    <t>Parts for RFID</t>
-  </si>
-  <si>
     <t>CanaKit Raspberry Pi 3 Complete Starter Kit</t>
   </si>
   <si>
     <t>CanaKit</t>
   </si>
   <si>
-    <t>MFRC522 RFID Sensor Module</t>
-  </si>
-  <si>
-    <t>https://www.amazon.ca/CanaKit-Raspberry-Ultimate-Starter-Kit/dp/B01CCF9BYG/ref=sr_1_3?ie=UTF8&amp;qid=1506104637&amp;sr=8-3&amp;keywords=sense+hat</t>
-  </si>
-  <si>
-    <t>https://www.amazon.ca/SainSmart-101-50-141-Mifare-Antenna-Proximity/dp/B00E37T2F0/ref=sr_1_2?ie=UTF8&amp;qid=1506622441&amp;sr=8-2&amp;keywords=rfid+rc522</t>
-  </si>
-  <si>
     <t>Parts</t>
   </si>
   <si>
     <t>SainSmart</t>
   </si>
   <si>
-    <t>Provides Raspberry Pi 3 Ultimate Kit that includes jump wires, breadboard, LEDs, resistors, etc…</t>
-  </si>
-  <si>
-    <t>RC522 Card Reader with an antenna. Comes with a reader card for the proximity sensor.</t>
-  </si>
-  <si>
-    <t>Total after taxes + shipping</t>
-  </si>
-  <si>
-    <t>LCD screen to display the text from the RFID</t>
-  </si>
-  <si>
-    <t>https://www.amazon.ca/SainSmart-Module-Arduino-Board-White/dp/B003B22UR0/ref=sr_1_5?s=electronics&amp;ie=UTF8&amp;qid=1506705910&amp;sr=1-5&amp;keywords=LCD+1602</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20x4 LCD Module </t>
+    <t>Part #</t>
+  </si>
+  <si>
+    <t>Grand Total (Incl. taxes)</t>
+  </si>
+  <si>
+    <t>Shipping</t>
+  </si>
+  <si>
+    <t>Estimated GST/HST</t>
+  </si>
+  <si>
+    <t>RFID Sensor Module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20x4 IIC/I2C/TWI LCD Module </t>
+  </si>
+  <si>
+    <t>Ruel John Cootauco - Parts List for RFID</t>
+  </si>
+  <si>
+    <t>Resources</t>
+  </si>
+  <si>
+    <t>https://www.amazon.ca/gp/product/B01CCF9BYG/ref=ox_sc_sfl_image_1?ie=UTF8&amp;psc=1&amp;smid=A34IVHW5OUAV7P</t>
+  </si>
+  <si>
+    <t>https://www.amazon.ca/gp/product/B003B22UR0/ref=ox_sc_sfl_image_3?ie=UTF8&amp;psc=1&amp;smid=A1CJB5SYI9X4XC</t>
+  </si>
+  <si>
+    <t>https://www.amazon.ca/gp/product/B00E37T2F0/ref=ox_sc_sfl_image_2?ie=UTF8&amp;psc=1&amp;smid=A1CJB5SYI9X4XC</t>
+  </si>
+  <si>
+    <t>Unit Cost</t>
+  </si>
+  <si>
+    <t>LCD screen to display the data read from the RFID tag/card.</t>
+  </si>
+  <si>
+    <t>RFID sensor that will read RFID tags 
+&amp; cards when near the proximity sensor.</t>
+  </si>
+  <si>
+    <t>Raspberry Pi including environment
+tools for development.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">               FREE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.000"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="00000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,18 +151,70 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -160,7 +230,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -174,7 +244,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -183,6 +252,27 @@
     </xf>
     <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -470,17 +560,17 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -488,231 +578,304 @@
     <col min="10" max="10" width="61.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+    </row>
+    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+    </row>
+    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="93.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="20">
+        <v>682710991511</v>
+      </c>
+      <c r="E4" s="30">
+        <v>119.99</v>
+      </c>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:8" ht="131.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1">
-        <v>119.99</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C5" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="20">
+        <v>10150141</v>
+      </c>
+      <c r="E5" s="30">
+        <v>15</v>
+      </c>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="1:8" ht="93.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1">
-        <v>15</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="B6" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="21">
+        <v>20011913</v>
+      </c>
+      <c r="E6" s="30">
         <v>19.989999999999998</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="14"/>
       <c r="G6" s="1"/>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+    <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="14"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1">
+    <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="18"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="19">
         <v>154.97999999999999</v>
       </c>
+      <c r="F8" s="14"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1">
-        <v>175.13</v>
-      </c>
+    <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19">
+        <v>15.6</v>
+      </c>
+      <c r="F9" s="14"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="13"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+    <row r="10" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12"/>
+    </row>
+    <row r="11" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="18"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="19">
+        <v>170.58</v>
+      </c>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="23"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C25" s="9"/>
       <c r="E25" s="5"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C26" s="9"/>
       <c r="E26" s="5"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C27" s="9"/>
       <c r="E27" s="5"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C28" s="9"/>
       <c r="E28" s="5"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C29" s="9"/>
       <c r="E29" s="5"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C30" s="9"/>
       <c r="E30" s="5"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C31" s="9"/>
       <c r="E31" s="5"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C32" s="9"/>
       <c r="E32" s="5"/>
       <c r="G32" s="6"/>
@@ -809,13 +972,13 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="13"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="12"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -825,12 +988,12 @@
     <mergeCell ref="G12:H12"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1"/>
-    <hyperlink ref="E4" r:id="rId2"/>
-    <hyperlink ref="E6" r:id="rId3"/>
+    <hyperlink ref="A15" r:id="rId1"/>
+    <hyperlink ref="A16" r:id="rId2"/>
+    <hyperlink ref="A14" r:id="rId3"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="65" orientation="landscape" r:id="rId4"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="60" fitToHeight="0" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed blog weekly dates and Week 7
Weeks shown were inaccurate, week 7 minor update.
</commit_message>
<xml_diff>
--- a/documentation/BudgetPlan.xlsx
+++ b/documentation/BudgetPlan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n01114847\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ceng317\SensorEffector\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,75 +24,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Link</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
-    <t>CAD$ Unit Cost</t>
-  </si>
-  <si>
     <t>Total for parts from CAD sources</t>
   </si>
   <si>
-    <t>Parts for RFID</t>
-  </si>
-  <si>
     <t>CanaKit Raspberry Pi 3 Complete Starter Kit</t>
   </si>
   <si>
     <t>CanaKit</t>
   </si>
   <si>
-    <t>MFRC522 RFID Sensor Module</t>
-  </si>
-  <si>
-    <t>https://www.amazon.ca/CanaKit-Raspberry-Ultimate-Starter-Kit/dp/B01CCF9BYG/ref=sr_1_3?ie=UTF8&amp;qid=1506104637&amp;sr=8-3&amp;keywords=sense+hat</t>
-  </si>
-  <si>
-    <t>https://www.amazon.ca/SainSmart-101-50-141-Mifare-Antenna-Proximity/dp/B00E37T2F0/ref=sr_1_2?ie=UTF8&amp;qid=1506622441&amp;sr=8-2&amp;keywords=rfid+rc522</t>
-  </si>
-  <si>
     <t>Parts</t>
   </si>
   <si>
     <t>SainSmart</t>
   </si>
   <si>
-    <t>Provides Raspberry Pi 3 Ultimate Kit that includes jump wires, breadboard, LEDs, resistors, etc…</t>
-  </si>
-  <si>
-    <t>RC522 Card Reader with an antenna. Comes with a reader card for the proximity sensor.</t>
-  </si>
-  <si>
-    <t>Total after taxes + shipping</t>
-  </si>
-  <si>
-    <t>LCD screen to display the text from the RFID</t>
-  </si>
-  <si>
-    <t>https://www.amazon.ca/SainSmart-Module-Arduino-Board-White/dp/B003B22UR0/ref=sr_1_5?s=electronics&amp;ie=UTF8&amp;qid=1506705910&amp;sr=1-5&amp;keywords=LCD+1602</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20x4 LCD Module </t>
+    <t>Part #</t>
+  </si>
+  <si>
+    <t>Grand Total (Incl. taxes)</t>
+  </si>
+  <si>
+    <t>Shipping</t>
+  </si>
+  <si>
+    <t>Estimated GST/HST</t>
+  </si>
+  <si>
+    <t>RFID Sensor Module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20x4 IIC/I2C/TWI LCD Module </t>
+  </si>
+  <si>
+    <t>Ruel John Cootauco - Parts List for RFID</t>
+  </si>
+  <si>
+    <t>Resources</t>
+  </si>
+  <si>
+    <t>https://www.amazon.ca/gp/product/B01CCF9BYG/ref=ox_sc_sfl_image_1?ie=UTF8&amp;psc=1&amp;smid=A34IVHW5OUAV7P</t>
+  </si>
+  <si>
+    <t>https://www.amazon.ca/gp/product/B003B22UR0/ref=ox_sc_sfl_image_3?ie=UTF8&amp;psc=1&amp;smid=A1CJB5SYI9X4XC</t>
+  </si>
+  <si>
+    <t>https://www.amazon.ca/gp/product/B00E37T2F0/ref=ox_sc_sfl_image_2?ie=UTF8&amp;psc=1&amp;smid=A1CJB5SYI9X4XC</t>
+  </si>
+  <si>
+    <t>Unit Cost</t>
+  </si>
+  <si>
+    <t>LCD screen to display the data read from the RFID tag/card.</t>
+  </si>
+  <si>
+    <t>RFID sensor that will read RFID tags 
+&amp; cards when near the proximity sensor.</t>
+  </si>
+  <si>
+    <t>Raspberry Pi including environment
+tools for development.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">               FREE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.000"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="00000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,18 +151,70 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -160,7 +230,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -174,7 +244,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -183,6 +252,27 @@
     </xf>
     <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -470,17 +560,17 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -488,231 +578,304 @@
     <col min="10" max="10" width="61.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+    </row>
+    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+    </row>
+    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="93.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="20">
+        <v>682710991511</v>
+      </c>
+      <c r="E4" s="30">
+        <v>119.99</v>
+      </c>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:8" ht="131.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1">
-        <v>119.99</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C5" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="20">
+        <v>10150141</v>
+      </c>
+      <c r="E5" s="30">
+        <v>15</v>
+      </c>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="1:8" ht="93.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1">
-        <v>15</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="B6" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="21">
+        <v>20011913</v>
+      </c>
+      <c r="E6" s="30">
         <v>19.989999999999998</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="14"/>
       <c r="G6" s="1"/>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+    <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="14"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1">
+    <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="18"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="19">
         <v>154.97999999999999</v>
       </c>
+      <c r="F8" s="14"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1">
-        <v>175.13</v>
-      </c>
+    <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19">
+        <v>15.6</v>
+      </c>
+      <c r="F9" s="14"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="13"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+    <row r="10" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12"/>
+    </row>
+    <row r="11" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="18"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="19">
+        <v>170.58</v>
+      </c>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="23"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C25" s="9"/>
       <c r="E25" s="5"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C26" s="9"/>
       <c r="E26" s="5"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C27" s="9"/>
       <c r="E27" s="5"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C28" s="9"/>
       <c r="E28" s="5"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C29" s="9"/>
       <c r="E29" s="5"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C30" s="9"/>
       <c r="E30" s="5"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C31" s="9"/>
       <c r="E31" s="5"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C32" s="9"/>
       <c r="E32" s="5"/>
       <c r="G32" s="6"/>
@@ -809,13 +972,13 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="13"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="12"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -825,12 +988,12 @@
     <mergeCell ref="G12:H12"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1"/>
-    <hyperlink ref="E4" r:id="rId2"/>
-    <hyperlink ref="E6" r:id="rId3"/>
+    <hyperlink ref="A15" r:id="rId1"/>
+    <hyperlink ref="A16" r:id="rId2"/>
+    <hyperlink ref="A14" r:id="rId3"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="65" orientation="landscape" r:id="rId4"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="60" fitToHeight="0" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>